<commit_message>
update to the experiment chart
</commit_message>
<xml_diff>
--- a/cw ismir2014/cw_ismir2014_experiments.xlsx
+++ b/cw ismir2014/cw_ismir2014_experiments.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="69">
   <si>
     <t>Precision</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -247,6 +247,50 @@
   </si>
   <si>
     <t>[0.12, 0.12, 0.12]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>median threshold, converge =&gt; 0.001</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>filtering</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>high pass only</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DR1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DR1 (de-outliers)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DR1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DR2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DR2 (de-outliers)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DR3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DR3 (de-outliers)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>high pass 8000 and low pass 8000</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -306,7 +350,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -328,6 +372,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -458,7 +508,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="273">
+  <cellStyleXfs count="423">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -732,8 +782,158 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -771,8 +971,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="273">
+  <cellStyles count="423">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="已瀏覽過的超連結" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="已瀏覽過的超連結" xfId="4" builtinId="9" hidden="1"/>
@@ -910,6 +1111,81 @@
     <cellStyle name="已瀏覽過的超連結" xfId="268" builtinId="9" hidden="1"/>
     <cellStyle name="已瀏覽過的超連結" xfId="270" builtinId="9" hidden="1"/>
     <cellStyle name="已瀏覽過的超連結" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="324" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="326" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="328" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="330" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="332" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="334" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="336" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="344" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="346" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="348" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="362" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="364" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="366" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="368" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="370" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="372" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="374" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="376" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="378" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="380" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="382" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="384" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="386" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="388" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="390" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="392" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="394" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="396" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="398" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="400" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="402" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="404" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="406" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="408" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="410" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="412" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="414" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="416" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="418" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="420" builtinId="9" hidden="1"/>
+    <cellStyle name="已瀏覽過的超連結" xfId="422" builtinId="9" hidden="1"/>
     <cellStyle name="超連結" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超連結" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="超連結" xfId="5" builtinId="8" hidden="1"/>
@@ -1046,6 +1322,81 @@
     <cellStyle name="超連結" xfId="267" builtinId="8" hidden="1"/>
     <cellStyle name="超連結" xfId="269" builtinId="8" hidden="1"/>
     <cellStyle name="超連結" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="321" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="323" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="325" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="327" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="329" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="331" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="333" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="335" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="337" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="339" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="341" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="343" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="345" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="347" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="349" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="351" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="353" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="359" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="361" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="363" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="365" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="367" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="369" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="371" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="373" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="375" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="377" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="379" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="381" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="383" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="385" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="387" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="389" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="391" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="393" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="395" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="397" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="399" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="401" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="403" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="405" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="407" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="409" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="411" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="413" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="415" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="417" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="419" builtinId="8" hidden="1"/>
+    <cellStyle name="超連結" xfId="421" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1374,10 +1725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I106"/>
+  <dimension ref="A1:I211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D111" sqref="D111"/>
+    <sheetView tabSelected="1" topLeftCell="A175" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C203" sqref="C203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3030,6 +3381,1558 @@
         <v>0.61848518845937484</v>
       </c>
     </row>
+    <row r="108" spans="2:9">
+      <c r="B108" t="s">
+        <v>50</v>
+      </c>
+      <c r="C108" s="6">
+        <v>64</v>
+      </c>
+      <c r="D108" t="s">
+        <v>57</v>
+      </c>
+      <c r="E108" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F108">
+        <v>0.54669999999999996</v>
+      </c>
+      <c r="G108">
+        <v>0.6895</v>
+      </c>
+      <c r="H108" s="23">
+        <f t="shared" ref="H108:H110" si="13">2*F108*G108/(F108+G108)</f>
+        <v>0.6098522083805209</v>
+      </c>
+      <c r="I108" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="109" spans="2:9">
+      <c r="D109" t="s">
+        <v>52</v>
+      </c>
+      <c r="E109" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F109">
+        <v>0.69079999999999997</v>
+      </c>
+      <c r="G109">
+        <v>0.82540000000000002</v>
+      </c>
+      <c r="H109" s="23">
+        <f t="shared" si="13"/>
+        <v>0.75212547157367105</v>
+      </c>
+    </row>
+    <row r="110" spans="2:9">
+      <c r="E110" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F110">
+        <v>0.56599999999999995</v>
+      </c>
+      <c r="G110">
+        <v>0.4758</v>
+      </c>
+      <c r="H110" s="23">
+        <f t="shared" si="13"/>
+        <v>0.51699520061432136</v>
+      </c>
+    </row>
+    <row r="112" spans="2:9">
+      <c r="B112" t="s">
+        <v>53</v>
+      </c>
+      <c r="C112" s="6">
+        <v>53</v>
+      </c>
+      <c r="D112" t="s">
+        <v>57</v>
+      </c>
+      <c r="E112" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F112">
+        <v>0.60550000000000004</v>
+      </c>
+      <c r="G112">
+        <v>0.71319999999999995</v>
+      </c>
+      <c r="H112" s="23">
+        <f t="shared" ref="H112:H114" si="14">2*F112*G112/(F112+G112)</f>
+        <v>0.65495199818002581</v>
+      </c>
+      <c r="I112" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="113" spans="2:9">
+      <c r="D113" t="s">
+        <v>52</v>
+      </c>
+      <c r="E113" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F113">
+        <v>0.72350000000000003</v>
+      </c>
+      <c r="G113">
+        <v>0.83709999999999996</v>
+      </c>
+      <c r="H113" s="23">
+        <f t="shared" si="14"/>
+        <v>0.77616538510829169</v>
+      </c>
+    </row>
+    <row r="114" spans="2:9">
+      <c r="E114" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F114">
+        <v>0.6784</v>
+      </c>
+      <c r="G114">
+        <v>0.56679999999999997</v>
+      </c>
+      <c r="H114" s="23">
+        <f t="shared" si="14"/>
+        <v>0.61759897205268222</v>
+      </c>
+    </row>
+    <row r="116" spans="2:9">
+      <c r="B116" t="s">
+        <v>50</v>
+      </c>
+      <c r="C116" s="6">
+        <v>64</v>
+      </c>
+      <c r="D116" t="s">
+        <v>57</v>
+      </c>
+      <c r="E116" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F116">
+        <v>0.62339999999999995</v>
+      </c>
+      <c r="G116">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="H116" s="23">
+        <f t="shared" ref="H116:H118" si="15">2*F116*G116/(F116+G116)</f>
+        <v>0.66301216764308246</v>
+      </c>
+      <c r="I116" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="117" spans="2:9">
+      <c r="D117" t="s">
+        <v>52</v>
+      </c>
+      <c r="E117" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F117">
+        <v>0.60150000000000003</v>
+      </c>
+      <c r="G117">
+        <v>0.84350000000000003</v>
+      </c>
+      <c r="H117" s="23">
+        <f t="shared" si="15"/>
+        <v>0.70223564013840845</v>
+      </c>
+    </row>
+    <row r="118" spans="2:9">
+      <c r="E118" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F118">
+        <v>0.46579999999999999</v>
+      </c>
+      <c r="G118">
+        <v>0.50190000000000001</v>
+      </c>
+      <c r="H118" s="23">
+        <f t="shared" si="15"/>
+        <v>0.48317664565464508</v>
+      </c>
+    </row>
+    <row r="120" spans="2:9">
+      <c r="B120" t="s">
+        <v>53</v>
+      </c>
+      <c r="C120" s="6">
+        <v>53</v>
+      </c>
+      <c r="D120" t="s">
+        <v>57</v>
+      </c>
+      <c r="E120" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F120">
+        <v>0.67110000000000003</v>
+      </c>
+      <c r="G120">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="H120" s="23">
+        <f t="shared" ref="H120:H163" si="16">2*F120*G120/(F120+G120)</f>
+        <v>0.70273498509158039</v>
+      </c>
+      <c r="I120" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="121" spans="2:9">
+      <c r="D121" t="s">
+        <v>52</v>
+      </c>
+      <c r="E121" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F121">
+        <v>0.66220000000000001</v>
+      </c>
+      <c r="G121">
+        <v>0.85519999999999996</v>
+      </c>
+      <c r="H121" s="23">
+        <f t="shared" si="16"/>
+        <v>0.74642604454988792</v>
+      </c>
+    </row>
+    <row r="122" spans="2:9">
+      <c r="E122" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F122">
+        <v>0.59109999999999996</v>
+      </c>
+      <c r="G122">
+        <v>0.58340000000000003</v>
+      </c>
+      <c r="H122" s="23">
+        <f t="shared" si="16"/>
+        <v>0.58722475947211572</v>
+      </c>
+    </row>
+    <row r="124" spans="2:9">
+      <c r="B124" t="s">
+        <v>50</v>
+      </c>
+      <c r="C124" s="6">
+        <v>64</v>
+      </c>
+      <c r="D124" t="s">
+        <v>57</v>
+      </c>
+      <c r="E124" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F124">
+        <v>0.61919999999999997</v>
+      </c>
+      <c r="G124">
+        <v>0.70640000000000003</v>
+      </c>
+      <c r="H124" s="23">
+        <f t="shared" si="16"/>
+        <v>0.65993192516596255</v>
+      </c>
+      <c r="I124" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="125" spans="2:9">
+      <c r="D125" t="s">
+        <v>52</v>
+      </c>
+      <c r="E125" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F125">
+        <v>0.70799999999999996</v>
+      </c>
+      <c r="G125">
+        <v>0.82569999999999999</v>
+      </c>
+      <c r="H125" s="23">
+        <f t="shared" si="16"/>
+        <v>0.76233370281019752</v>
+      </c>
+    </row>
+    <row r="126" spans="2:9">
+      <c r="E126" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F126">
+        <v>0.55349999999999999</v>
+      </c>
+      <c r="G126">
+        <v>0.4793</v>
+      </c>
+      <c r="H126" s="23">
+        <f t="shared" si="16"/>
+        <v>0.51373460495739742</v>
+      </c>
+    </row>
+    <row r="128" spans="2:9">
+      <c r="B128" t="s">
+        <v>53</v>
+      </c>
+      <c r="C128" s="6">
+        <v>53</v>
+      </c>
+      <c r="D128" t="s">
+        <v>57</v>
+      </c>
+      <c r="E128" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F128">
+        <v>0.67530000000000001</v>
+      </c>
+      <c r="G128">
+        <v>0.7369</v>
+      </c>
+      <c r="H128" s="23">
+        <f t="shared" si="16"/>
+        <v>0.7047565075768305</v>
+      </c>
+      <c r="I128" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9">
+      <c r="D129" t="s">
+        <v>52</v>
+      </c>
+      <c r="E129" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F129">
+        <v>0.74080000000000001</v>
+      </c>
+      <c r="G129">
+        <v>0.83930000000000005</v>
+      </c>
+      <c r="H129" s="23">
+        <f t="shared" si="16"/>
+        <v>0.78697986203404846</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9">
+      <c r="E130" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F130">
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="G130">
+        <v>0.5696</v>
+      </c>
+      <c r="H130" s="23">
+        <f t="shared" si="16"/>
+        <v>0.61825561978163135</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9">
+      <c r="E131" s="4"/>
+      <c r="H131" s="23"/>
+    </row>
+    <row r="132" spans="1:9">
+      <c r="B132" t="s">
+        <v>50</v>
+      </c>
+      <c r="C132" s="6">
+        <v>64</v>
+      </c>
+      <c r="D132" t="s">
+        <v>57</v>
+      </c>
+      <c r="E132" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F132">
+        <v>0.62109999999999999</v>
+      </c>
+      <c r="G132">
+        <v>0.7046</v>
+      </c>
+      <c r="H132" s="23">
+        <f t="shared" ref="H132:H134" si="17">2*F132*G132/(F132+G132)</f>
+        <v>0.66022035151240865</v>
+      </c>
+      <c r="I132" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9">
+      <c r="D133" t="s">
+        <v>52</v>
+      </c>
+      <c r="E133" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F133">
+        <v>0.69530000000000003</v>
+      </c>
+      <c r="G133">
+        <v>0.82909999999999995</v>
+      </c>
+      <c r="H133" s="23">
+        <f t="shared" si="17"/>
+        <v>0.75632803726056153</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9">
+      <c r="E134" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F134">
+        <v>0.46329999999999999</v>
+      </c>
+      <c r="G134">
+        <v>0.50729999999999997</v>
+      </c>
+      <c r="H134" s="23">
+        <f t="shared" si="17"/>
+        <v>0.484302678755409</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9">
+      <c r="B136" t="s">
+        <v>53</v>
+      </c>
+      <c r="C136" s="6">
+        <v>53</v>
+      </c>
+      <c r="D136" t="s">
+        <v>57</v>
+      </c>
+      <c r="E136" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F136">
+        <v>0.67759999999999998</v>
+      </c>
+      <c r="G136">
+        <v>0.73350000000000004</v>
+      </c>
+      <c r="H136" s="23">
+        <f t="shared" ref="H136:H138" si="18">2*F136*G136/(F136+G136)</f>
+        <v>0.70444277513996167</v>
+      </c>
+      <c r="I136" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9">
+      <c r="D137" t="s">
+        <v>52</v>
+      </c>
+      <c r="E137" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F137">
+        <v>0.73040000000000005</v>
+      </c>
+      <c r="G137">
+        <v>0.83889999999999998</v>
+      </c>
+      <c r="H137" s="23">
+        <f t="shared" si="18"/>
+        <v>0.78089920346651365</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9">
+      <c r="E138" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F138">
+        <v>0.54820000000000002</v>
+      </c>
+      <c r="G138">
+        <v>0.59319999999999995</v>
+      </c>
+      <c r="H138" s="23">
+        <f t="shared" si="18"/>
+        <v>0.56981293148764667</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9">
+      <c r="E139" s="4"/>
+      <c r="H139" s="23"/>
+    </row>
+    <row r="140" spans="1:9">
+      <c r="A140" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C140" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E140" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F140" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G140" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H140" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I140" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9">
+      <c r="A141" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B141" t="s">
+        <v>61</v>
+      </c>
+      <c r="C141" s="6">
+        <v>21</v>
+      </c>
+      <c r="D141" t="s">
+        <v>57</v>
+      </c>
+      <c r="E141" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F141">
+        <v>0.65820000000000001</v>
+      </c>
+      <c r="G141">
+        <v>0.64890000000000003</v>
+      </c>
+      <c r="H141" s="23">
+        <f t="shared" si="16"/>
+        <v>0.6535169153086986</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9">
+      <c r="D142" t="s">
+        <v>52</v>
+      </c>
+      <c r="E142" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F142">
+        <v>0.50160000000000005</v>
+      </c>
+      <c r="G142">
+        <v>0.39369999999999999</v>
+      </c>
+      <c r="H142" s="23">
+        <f t="shared" si="16"/>
+        <v>0.44114803976320788</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9">
+      <c r="E143" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F143">
+        <v>0.58179999999999998</v>
+      </c>
+      <c r="G143">
+        <v>0.41649999999999998</v>
+      </c>
+      <c r="H143" s="23">
+        <f t="shared" si="16"/>
+        <v>0.485464689972954</v>
+      </c>
+    </row>
+    <row r="145" spans="2:8">
+      <c r="B145" t="s">
+        <v>62</v>
+      </c>
+      <c r="C145" s="6">
+        <v>20</v>
+      </c>
+      <c r="D145" t="s">
+        <v>57</v>
+      </c>
+      <c r="E145" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F145">
+        <v>0.66259999999999997</v>
+      </c>
+      <c r="G145">
+        <v>0.67030000000000001</v>
+      </c>
+      <c r="H145" s="23">
+        <f t="shared" si="16"/>
+        <v>0.66642775902168194</v>
+      </c>
+    </row>
+    <row r="146" spans="2:8">
+      <c r="D146" t="s">
+        <v>52</v>
+      </c>
+      <c r="E146" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F146">
+        <v>0.62</v>
+      </c>
+      <c r="G146">
+        <v>0.39329999999999998</v>
+      </c>
+      <c r="H146" s="23">
+        <f t="shared" si="16"/>
+        <v>0.48129083193526095</v>
+      </c>
+    </row>
+    <row r="147" spans="2:8">
+      <c r="E147" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F147">
+        <v>0.6391</v>
+      </c>
+      <c r="G147">
+        <v>0.54610000000000003</v>
+      </c>
+      <c r="H147" s="23">
+        <f t="shared" si="16"/>
+        <v>0.58895124873439075</v>
+      </c>
+    </row>
+    <row r="149" spans="2:8">
+      <c r="B149" t="s">
+        <v>64</v>
+      </c>
+      <c r="C149" s="6">
+        <v>22</v>
+      </c>
+      <c r="D149" t="s">
+        <v>57</v>
+      </c>
+      <c r="E149" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F149">
+        <v>0.59360000000000002</v>
+      </c>
+      <c r="G149">
+        <v>0.69110000000000005</v>
+      </c>
+      <c r="H149" s="23">
+        <f t="shared" si="16"/>
+        <v>0.63865020627383828</v>
+      </c>
+    </row>
+    <row r="150" spans="2:8">
+      <c r="D150" t="s">
+        <v>52</v>
+      </c>
+      <c r="E150" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F150">
+        <v>0.73850000000000005</v>
+      </c>
+      <c r="G150">
+        <v>0.90349999999999997</v>
+      </c>
+      <c r="H150" s="23">
+        <f t="shared" si="16"/>
+        <v>0.81270980511571256</v>
+      </c>
+    </row>
+    <row r="151" spans="2:8">
+      <c r="E151" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F151">
+        <v>0.6744</v>
+      </c>
+      <c r="G151">
+        <v>0.49380000000000002</v>
+      </c>
+      <c r="H151" s="23">
+        <f t="shared" si="16"/>
+        <v>0.57013990755007693</v>
+      </c>
+    </row>
+    <row r="153" spans="2:8">
+      <c r="B153" t="s">
+        <v>65</v>
+      </c>
+      <c r="C153" s="6">
+        <v>17</v>
+      </c>
+      <c r="D153" t="s">
+        <v>57</v>
+      </c>
+      <c r="E153" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F153">
+        <v>0.62190000000000001</v>
+      </c>
+      <c r="G153">
+        <v>0.74970000000000003</v>
+      </c>
+      <c r="H153" s="23">
+        <f t="shared" si="16"/>
+        <v>0.67984606299212602</v>
+      </c>
+    </row>
+    <row r="154" spans="2:8">
+      <c r="D154" t="s">
+        <v>52</v>
+      </c>
+      <c r="E154" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F154">
+        <v>0.78190000000000004</v>
+      </c>
+      <c r="G154">
+        <v>0.91439999999999999</v>
+      </c>
+      <c r="H154" s="23">
+        <f t="shared" si="16"/>
+        <v>0.84297513411542768</v>
+      </c>
+    </row>
+    <row r="155" spans="2:8">
+      <c r="E155" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F155">
+        <v>0.80030000000000001</v>
+      </c>
+      <c r="G155">
+        <v>0.60809999999999997</v>
+      </c>
+      <c r="H155" s="23">
+        <f t="shared" si="16"/>
+        <v>0.69108552967906844</v>
+      </c>
+    </row>
+    <row r="157" spans="2:8">
+      <c r="B157" t="s">
+        <v>66</v>
+      </c>
+      <c r="C157" s="6">
+        <v>21</v>
+      </c>
+      <c r="D157" t="s">
+        <v>57</v>
+      </c>
+      <c r="E157" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F157">
+        <v>0.50719999999999998</v>
+      </c>
+      <c r="G157">
+        <v>0.67620000000000002</v>
+      </c>
+      <c r="H157" s="23">
+        <f t="shared" si="16"/>
+        <v>0.57963265168159539</v>
+      </c>
+    </row>
+    <row r="158" spans="2:8">
+      <c r="D158" t="s">
+        <v>52</v>
+      </c>
+      <c r="E158" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F158">
+        <v>0.7782</v>
+      </c>
+      <c r="G158">
+        <v>0.88690000000000002</v>
+      </c>
+      <c r="H158" s="23">
+        <f t="shared" si="16"/>
+        <v>0.8290019578403699</v>
+      </c>
+    </row>
+    <row r="159" spans="2:8">
+      <c r="E159" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F159">
+        <v>0.50439999999999996</v>
+      </c>
+      <c r="G159">
+        <v>0.47989999999999999</v>
+      </c>
+      <c r="H159" s="23">
+        <f t="shared" si="16"/>
+        <v>0.49184508787971143</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8">
+      <c r="B161" t="s">
+        <v>67</v>
+      </c>
+      <c r="C161" s="6">
+        <v>20</v>
+      </c>
+      <c r="D161" t="s">
+        <v>57</v>
+      </c>
+      <c r="E161" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F161">
+        <v>0.56459999999999999</v>
+      </c>
+      <c r="G161">
+        <v>0.69279999999999997</v>
+      </c>
+      <c r="H161" s="23">
+        <f t="shared" si="16"/>
+        <v>0.6221645936058533</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8">
+      <c r="D162" t="s">
+        <v>52</v>
+      </c>
+      <c r="E162" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F162">
+        <v>0.85029999999999994</v>
+      </c>
+      <c r="G162">
+        <v>0.90029999999999999</v>
+      </c>
+      <c r="H162" s="23">
+        <f t="shared" si="16"/>
+        <v>0.87458595909973713</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8">
+      <c r="E163" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F163">
+        <v>0.58940000000000003</v>
+      </c>
+      <c r="G163">
+        <v>0.48730000000000001</v>
+      </c>
+      <c r="H163" s="23">
+        <f t="shared" si="16"/>
+        <v>0.53350909259775248</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8">
+      <c r="A165" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="B165" t="s">
+        <v>61</v>
+      </c>
+      <c r="C165" s="6">
+        <v>21</v>
+      </c>
+      <c r="D165" t="s">
+        <v>57</v>
+      </c>
+      <c r="E165" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F165">
+        <v>0.62639999999999996</v>
+      </c>
+      <c r="G165">
+        <v>0.64939999999999998</v>
+      </c>
+      <c r="H165" s="23">
+        <f t="shared" ref="H165:H187" si="19">2*F165*G165/(F165+G165)</f>
+        <v>0.63769267910330774</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8">
+      <c r="D166" t="s">
+        <v>52</v>
+      </c>
+      <c r="E166" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F166">
+        <v>0.4607</v>
+      </c>
+      <c r="G166">
+        <v>0.58320000000000005</v>
+      </c>
+      <c r="H166" s="23">
+        <f t="shared" si="19"/>
+        <v>0.5147624101925472</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8">
+      <c r="E167" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F167">
+        <v>0.55479999999999996</v>
+      </c>
+      <c r="G167">
+        <v>0.3977</v>
+      </c>
+      <c r="H167" s="23">
+        <f t="shared" si="19"/>
+        <v>0.46329440419947504</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8">
+      <c r="B169" t="s">
+        <v>62</v>
+      </c>
+      <c r="C169" s="6">
+        <v>20</v>
+      </c>
+      <c r="D169" t="s">
+        <v>57</v>
+      </c>
+      <c r="E169" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F169">
+        <v>0.6613</v>
+      </c>
+      <c r="G169">
+        <v>0.6673</v>
+      </c>
+      <c r="H169" s="23">
+        <f t="shared" ref="H169:H187" si="20">2*F169*G169/(F169+G169)</f>
+        <v>0.66428645190426017</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8">
+      <c r="D170" t="s">
+        <v>52</v>
+      </c>
+      <c r="E170" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F170">
+        <v>0.46639999999999998</v>
+      </c>
+      <c r="G170">
+        <v>0.60299999999999998</v>
+      </c>
+      <c r="H170" s="23">
+        <f t="shared" si="20"/>
+        <v>0.52597568730129041</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8">
+      <c r="E171" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F171">
+        <v>0.62539999999999996</v>
+      </c>
+      <c r="G171">
+        <v>0.55049999999999999</v>
+      </c>
+      <c r="H171" s="23">
+        <f t="shared" si="20"/>
+        <v>0.58556458882558038</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8">
+      <c r="B173" t="s">
+        <v>64</v>
+      </c>
+      <c r="C173" s="6">
+        <v>22</v>
+      </c>
+      <c r="D173" t="s">
+        <v>57</v>
+      </c>
+      <c r="E173" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F173">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="G173">
+        <v>0.69340000000000002</v>
+      </c>
+      <c r="H173" s="23">
+        <f t="shared" ref="H173:H187" si="21">2*F173*G173/(F173+G173)</f>
+        <v>0.62446678293959079</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8">
+      <c r="D174" t="s">
+        <v>52</v>
+      </c>
+      <c r="E174" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F174">
+        <v>0.84150000000000003</v>
+      </c>
+      <c r="G174">
+        <v>0.98519999999999996</v>
+      </c>
+      <c r="H174" s="23">
+        <f t="shared" si="21"/>
+        <v>0.90769781573328945</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8">
+      <c r="E175" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F175">
+        <v>0.70940000000000003</v>
+      </c>
+      <c r="G175">
+        <v>0.50080000000000002</v>
+      </c>
+      <c r="H175" s="23">
+        <f t="shared" si="21"/>
+        <v>0.58712199636423745</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8">
+      <c r="B177" t="s">
+        <v>65</v>
+      </c>
+      <c r="C177" s="6">
+        <v>17</v>
+      </c>
+      <c r="D177" t="s">
+        <v>57</v>
+      </c>
+      <c r="E177" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F177">
+        <v>0.60050000000000003</v>
+      </c>
+      <c r="G177">
+        <v>0.78759999999999997</v>
+      </c>
+      <c r="H177" s="23">
+        <f t="shared" ref="H177:H187" si="22">2*F177*G177/(F177+G177)</f>
+        <v>0.68144053022116557</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8">
+      <c r="D178" t="s">
+        <v>52</v>
+      </c>
+      <c r="E178" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F178">
+        <v>0.84619999999999995</v>
+      </c>
+      <c r="G178">
+        <v>0.98640000000000005</v>
+      </c>
+      <c r="H178" s="23">
+        <f t="shared" si="22"/>
+        <v>0.91093711666484778</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8">
+      <c r="E179" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F179">
+        <v>0.84989999999999999</v>
+      </c>
+      <c r="G179">
+        <v>0.62409999999999999</v>
+      </c>
+      <c r="H179" s="23">
+        <f t="shared" si="22"/>
+        <v>0.71970500678426053</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8">
+      <c r="B181" t="s">
+        <v>66</v>
+      </c>
+      <c r="C181" s="6">
+        <v>21</v>
+      </c>
+      <c r="D181" t="s">
+        <v>57</v>
+      </c>
+      <c r="E181" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F181">
+        <v>0.48870000000000002</v>
+      </c>
+      <c r="G181">
+        <v>0.70330000000000004</v>
+      </c>
+      <c r="H181" s="23">
+        <f t="shared" ref="H181:H187" si="23">2*F181*G181/(F181+G181)</f>
+        <v>0.57668239932885901</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8">
+      <c r="D182" t="s">
+        <v>52</v>
+      </c>
+      <c r="E182" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F182">
+        <v>0.6744</v>
+      </c>
+      <c r="G182">
+        <v>0.86109999999999998</v>
+      </c>
+      <c r="H182" s="23">
+        <f t="shared" si="23"/>
+        <v>0.75639966134809511</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8">
+      <c r="E183" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F183">
+        <v>0.44650000000000001</v>
+      </c>
+      <c r="G183">
+        <v>0.47139999999999999</v>
+      </c>
+      <c r="H183" s="23">
+        <f t="shared" si="23"/>
+        <v>0.45861226713149583</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8">
+      <c r="B185" t="s">
+        <v>67</v>
+      </c>
+      <c r="C185" s="6">
+        <v>20</v>
+      </c>
+      <c r="D185" t="s">
+        <v>57</v>
+      </c>
+      <c r="E185" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F185">
+        <v>0.54120000000000001</v>
+      </c>
+      <c r="G185">
+        <v>0.6996</v>
+      </c>
+      <c r="H185" s="23">
+        <f t="shared" ref="H185:H187" si="24">2*F185*G185/(F185+G185)</f>
+        <v>0.61028936170212755</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8">
+      <c r="D186" t="s">
+        <v>52</v>
+      </c>
+      <c r="E186" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F186">
+        <v>0.69989999999999997</v>
+      </c>
+      <c r="G186">
+        <v>0.85419999999999996</v>
+      </c>
+      <c r="H186" s="23">
+        <f t="shared" si="24"/>
+        <v>0.76939010359693705</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8">
+      <c r="E187" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F187">
+        <v>0.52900000000000003</v>
+      </c>
+      <c r="G187">
+        <v>0.48609999999999998</v>
+      </c>
+      <c r="H187" s="23">
+        <f t="shared" si="24"/>
+        <v>0.50664348340065024</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8">
+      <c r="A189" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="B189" t="s">
+        <v>61</v>
+      </c>
+      <c r="C189" s="6">
+        <v>21</v>
+      </c>
+      <c r="D189" t="s">
+        <v>57</v>
+      </c>
+      <c r="E189" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F189">
+        <v>0.58320000000000005</v>
+      </c>
+      <c r="G189">
+        <v>0.64449999999999996</v>
+      </c>
+      <c r="H189" s="23">
+        <f t="shared" ref="H189:H211" si="25">2*F189*G189/(F189+G189)</f>
+        <v>0.6123196220575059</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8">
+      <c r="D190" t="s">
+        <v>52</v>
+      </c>
+      <c r="E190" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F190">
+        <v>0.4955</v>
+      </c>
+      <c r="G190">
+        <v>0.58579999999999999</v>
+      </c>
+      <c r="H190" s="23">
+        <f t="shared" si="25"/>
+        <v>0.53687949690187742</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8">
+      <c r="E191" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F191">
+        <v>0.4335</v>
+      </c>
+      <c r="G191">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="H191" s="23">
+        <f t="shared" si="25"/>
+        <v>0.45284628099173552</v>
+      </c>
+    </row>
+    <row r="193" spans="2:8">
+      <c r="B193" t="s">
+        <v>62</v>
+      </c>
+      <c r="C193" s="6">
+        <v>20</v>
+      </c>
+      <c r="D193" t="s">
+        <v>57</v>
+      </c>
+      <c r="E193" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F193">
+        <v>0.61429999999999996</v>
+      </c>
+      <c r="G193">
+        <v>0.66039999999999999</v>
+      </c>
+      <c r="H193" s="23">
+        <f t="shared" ref="H193:H211" si="26">2*F193*G193/(F193+G193)</f>
+        <v>0.63651638816976541</v>
+      </c>
+    </row>
+    <row r="194" spans="2:8">
+      <c r="D194" t="s">
+        <v>52</v>
+      </c>
+      <c r="E194" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F194">
+        <v>0.50660000000000005</v>
+      </c>
+      <c r="G194">
+        <v>0.63660000000000005</v>
+      </c>
+      <c r="H194" s="23">
+        <f t="shared" si="26"/>
+        <v>0.56420846745976205</v>
+      </c>
+    </row>
+    <row r="195" spans="2:8">
+      <c r="E195" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F195">
+        <v>0.47699999999999998</v>
+      </c>
+      <c r="G195">
+        <v>0.5806</v>
+      </c>
+      <c r="H195" s="23">
+        <f t="shared" si="26"/>
+        <v>0.52372579425113464</v>
+      </c>
+    </row>
+    <row r="197" spans="2:8">
+      <c r="B197" t="s">
+        <v>64</v>
+      </c>
+      <c r="C197" s="6">
+        <v>22</v>
+      </c>
+      <c r="D197" t="s">
+        <v>57</v>
+      </c>
+      <c r="E197" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F197">
+        <v>0.5696</v>
+      </c>
+      <c r="G197">
+        <v>0.65949999999999998</v>
+      </c>
+      <c r="H197" s="23">
+        <f t="shared" ref="H197:H211" si="27">2*F197*G197/(F197+G197)</f>
+        <v>0.61126222439183142</v>
+      </c>
+    </row>
+    <row r="198" spans="2:8">
+      <c r="D198" t="s">
+        <v>52</v>
+      </c>
+      <c r="E198" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F198">
+        <v>0.84550000000000003</v>
+      </c>
+      <c r="G198">
+        <v>0.9546</v>
+      </c>
+      <c r="H198" s="23">
+        <f t="shared" si="27"/>
+        <v>0.89674384756402425</v>
+      </c>
+    </row>
+    <row r="199" spans="2:8">
+      <c r="E199" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F199">
+        <v>0.4829</v>
+      </c>
+      <c r="G199">
+        <v>0.49030000000000001</v>
+      </c>
+      <c r="H199" s="23">
+        <f t="shared" si="27"/>
+        <v>0.48657186600904234</v>
+      </c>
+    </row>
+    <row r="201" spans="2:8">
+      <c r="B201" t="s">
+        <v>65</v>
+      </c>
+      <c r="C201" s="6">
+        <v>17</v>
+      </c>
+      <c r="D201" t="s">
+        <v>57</v>
+      </c>
+      <c r="E201" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F201">
+        <v>0.59899999999999998</v>
+      </c>
+      <c r="G201">
+        <v>0.71760000000000002</v>
+      </c>
+      <c r="H201" s="23">
+        <f t="shared" ref="H201:H211" si="28">2*F201*G201/(F201+G201)</f>
+        <v>0.65295822573294848</v>
+      </c>
+    </row>
+    <row r="202" spans="2:8">
+      <c r="D202" t="s">
+        <v>52</v>
+      </c>
+      <c r="E202" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F202">
+        <v>0.86250000000000004</v>
+      </c>
+      <c r="G202">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="H202" s="23">
+        <f t="shared" si="28"/>
+        <v>0.91087551299589598</v>
+      </c>
+    </row>
+    <row r="203" spans="2:8">
+      <c r="E203" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F203">
+        <v>0.6159</v>
+      </c>
+      <c r="G203">
+        <v>0.59850000000000003</v>
+      </c>
+      <c r="H203" s="23">
+        <f t="shared" si="28"/>
+        <v>0.60707534584980249</v>
+      </c>
+    </row>
+    <row r="205" spans="2:8">
+      <c r="B205" t="s">
+        <v>66</v>
+      </c>
+      <c r="C205" s="6">
+        <v>21</v>
+      </c>
+      <c r="D205" t="s">
+        <v>57</v>
+      </c>
+      <c r="E205" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F205">
+        <v>0.45590000000000003</v>
+      </c>
+      <c r="G205">
+        <v>0.65529999999999999</v>
+      </c>
+      <c r="H205" s="23">
+        <f t="shared" ref="H205:H211" si="29">2*F205*G205/(F205+G205)</f>
+        <v>0.53770926925845941</v>
+      </c>
+    </row>
+    <row r="206" spans="2:8">
+      <c r="D206" t="s">
+        <v>52</v>
+      </c>
+      <c r="E206" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F206">
+        <v>0.76880000000000004</v>
+      </c>
+      <c r="G206">
+        <v>0.92649999999999999</v>
+      </c>
+      <c r="H206" s="23">
+        <f t="shared" si="29"/>
+        <v>0.84031522444405127</v>
+      </c>
+    </row>
+    <row r="207" spans="2:8">
+      <c r="E207" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F207">
+        <v>0.50270000000000004</v>
+      </c>
+      <c r="G207">
+        <v>0.53710000000000002</v>
+      </c>
+      <c r="H207" s="23">
+        <f t="shared" si="29"/>
+        <v>0.51933096749374885</v>
+      </c>
+    </row>
+    <row r="209" spans="2:8">
+      <c r="B209" t="s">
+        <v>67</v>
+      </c>
+      <c r="C209" s="6">
+        <v>20</v>
+      </c>
+      <c r="D209" t="s">
+        <v>57</v>
+      </c>
+      <c r="E209" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F209">
+        <v>0.52339999999999998</v>
+      </c>
+      <c r="G209">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="H209" s="23">
+        <f t="shared" ref="H209:H211" si="30">2*F209*G209/(F209+G209)</f>
+        <v>0.58961114819759686</v>
+      </c>
+    </row>
+    <row r="210" spans="2:8">
+      <c r="D210" t="s">
+        <v>52</v>
+      </c>
+      <c r="E210" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F210">
+        <v>0.80020000000000002</v>
+      </c>
+      <c r="G210">
+        <v>0.93210000000000004</v>
+      </c>
+      <c r="H210" s="23">
+        <f t="shared" si="30"/>
+        <v>0.86112846504647012</v>
+      </c>
+    </row>
+    <row r="211" spans="2:8">
+      <c r="E211" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F211">
+        <v>0.56459999999999999</v>
+      </c>
+      <c r="G211">
+        <v>0.53420000000000001</v>
+      </c>
+      <c r="H211" s="23">
+        <f t="shared" si="30"/>
+        <v>0.54897946851110302</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>